<commit_message>
agregar buscador a pdom y dlaborados
</commit_message>
<xml_diff>
--- a/Temp/Empleados_Ausentes.xlsx
+++ b/Temp/Empleados_Ausentes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="187">
   <si>
     <t>Empresa</t>
   </si>
@@ -32,6 +32,12 @@
     <t>Cantidad</t>
   </si>
   <si>
+    <t>JAVIER GARCIA GUTIERREZ</t>
+  </si>
+  <si>
+    <t>DELFINARIO</t>
+  </si>
+  <si>
     <t>EVARISTO CARDONA VILLA</t>
   </si>
   <si>
@@ -44,57 +50,102 @@
     <t>FOTO Y VIDEO</t>
   </si>
   <si>
-    <t>GUILLERMO ANTONIO PEREZ LOPEZ</t>
+    <t>JOSE LUIS CHICAS CASTELAN</t>
+  </si>
+  <si>
+    <t>CAMEL SAFARI</t>
+  </si>
+  <si>
+    <t>JESUS ANTONIO RUIZ COLLINS</t>
   </si>
   <si>
     <t>JUAN CARLOS ROSAS ALVAREZ</t>
   </si>
   <si>
+    <t>JOEL ISAAC RUIZ COLLINS</t>
+  </si>
+  <si>
+    <t>OLIVER ROBERTO HERNANDEZ MARTINEZ</t>
+  </si>
+  <si>
+    <t>CABO PULMO</t>
+  </si>
+  <si>
     <t>JONATHAN ULISES REYNOSO ORTEGA</t>
   </si>
   <si>
-    <t>CAMEL SAFARI</t>
+    <t>ABRAHAM OBED PEREZ AGUILAR</t>
   </si>
   <si>
     <t>CLAUDIA COLLINS GONZALEZ</t>
   </si>
   <si>
-    <t>MARCO ANTONIO BELMAR FERNANDEZ</t>
-  </si>
-  <si>
-    <t>FLYBOARD</t>
+    <t>LUCIA MARGARITA MAY RODRIGUEZ</t>
+  </si>
+  <si>
+    <t>TRANSPORTACION</t>
+  </si>
+  <si>
+    <t>LUIS MARTIN PEREZ MEDINA</t>
   </si>
   <si>
     <t>FELIPE FLORES BARRAGAN</t>
   </si>
   <si>
+    <t>JORDAN DE LA ROSA GONZALEZ</t>
+  </si>
+  <si>
+    <t>EDSON HUGO ESPINOZA MENDOZA</t>
+  </si>
+  <si>
+    <t>VELEROS</t>
+  </si>
+  <si>
+    <t>FERNANDO PLATA JIMENEZ</t>
+  </si>
+  <si>
     <t>LETICIA TORRES LUJAN</t>
   </si>
   <si>
     <t>FOTO CONCESIONES</t>
   </si>
   <si>
+    <t>JOSE EDUARDO VEGA DIAZ</t>
+  </si>
+  <si>
     <t>FABIAN GUTIERREZ DIAZ</t>
   </si>
   <si>
     <t>VENTAS CAD</t>
   </si>
   <si>
+    <t>DANIEL ALEJANDRO CARDENAS IBARRA</t>
+  </si>
+  <si>
+    <t>FELIX MARCIAL CAMPECHANO</t>
+  </si>
+  <si>
     <t>RAMON NAQUID REYES</t>
   </si>
   <si>
     <t xml:space="preserve">MARIA EUGENIA DEGREEF </t>
   </si>
   <si>
-    <t>DELFINARIO</t>
+    <t>FREDY ABARCA VALERIO</t>
+  </si>
+  <si>
+    <t>SEGURIDAD</t>
+  </si>
+  <si>
+    <t>JUAN ENRIQUE ZAMORA MENDOZA</t>
+  </si>
+  <si>
+    <t>FOTO Y VIDEO SJ</t>
   </si>
   <si>
     <t>JOEL CASTILLO CASTILLO</t>
   </si>
   <si>
-    <t>TRANSPORTACION</t>
-  </si>
-  <si>
     <t>FELIPE ENRIQUE FILIBERTO DIEZ CANEDO RUIZ</t>
   </si>
   <si>
@@ -110,12 +161,15 @@
     <t>JUAN EMILIO RODRIGUEZ ANDRADE</t>
   </si>
   <si>
+    <t xml:space="preserve">JOLEEN MARIANNE KOOPMANN </t>
+  </si>
+  <si>
+    <t>JONATHAN JIMENEZ AMILBURU</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANDREA RIZZI </t>
   </si>
   <si>
-    <t>VELEROS</t>
-  </si>
-  <si>
     <t>ANGELA PAOLA VIGUERAS GARCIA</t>
   </si>
   <si>
@@ -125,15 +179,27 @@
     <t>EMMANUEL ALEJANDRO HERRERA GARCIA</t>
   </si>
   <si>
-    <t>KARLA SOBEYDA MARTINEZ ROMERO</t>
-  </si>
-  <si>
     <t>MELINA GIZEH ARCE VAZQUEZ</t>
   </si>
   <si>
     <t>DANY PORTILLO CABRERA</t>
   </si>
   <si>
+    <t>GUILLERMO ALEJANDRO CANSECO HERNANDEZ</t>
+  </si>
+  <si>
+    <t>OFF ROAD</t>
+  </si>
+  <si>
+    <t>JESUS ALBERTO HERNANDEZ CRUZ</t>
+  </si>
+  <si>
+    <t>ANGEL DANIEL GUTIERREZ BELTRAN</t>
+  </si>
+  <si>
+    <t>MIGUEL ANGEL BRUNO CAMACHO MARTINEZ</t>
+  </si>
+  <si>
     <t>JOSE RAUL ROJAS DE LA PE/A</t>
   </si>
   <si>
@@ -143,6 +209,12 @@
     <t>BUCEO</t>
   </si>
   <si>
+    <t>JEENIFER ALEJANDRA CESE¥A JUAREZ</t>
+  </si>
+  <si>
+    <t>WHALE SHARK</t>
+  </si>
+  <si>
     <t>JAIRO JESUS ALONSO ONTIVEROS</t>
   </si>
   <si>
@@ -152,6 +224,9 @@
     <t>MIGUEL SANCHEZ GARCIA</t>
   </si>
   <si>
+    <t>JOSE RAMON AMADOR MONGES</t>
+  </si>
+  <si>
     <t>MAITE DIEZ CANEDO GUIJARRO</t>
   </si>
   <si>
@@ -164,6 +239,12 @@
     <t>CHRISTIAN ALEJANDRA NORIEGA JIMENEZ</t>
   </si>
   <si>
+    <t>ISAI BIBIANO LEYVA</t>
+  </si>
+  <si>
+    <t>MANTENIMIENTO CAD</t>
+  </si>
+  <si>
     <t>RUT ELENA HERNANDEZ PESCADOR</t>
   </si>
   <si>
@@ -179,19 +260,40 @@
     <t>MIGUEL ANGEL ESQUER SOTO</t>
   </si>
   <si>
-    <t>JUAN ABUNDIO ZAVALETA CORTEZ</t>
+    <t>JERSON JESERICK MENDOZA SALAZAR</t>
+  </si>
+  <si>
+    <t>OSCAR AGUILAR COLLINS</t>
   </si>
   <si>
     <t>CARLOS EZEQUIEL GONZALEZ CASTILLO</t>
   </si>
   <si>
-    <t>LILIA IMELDA MARTINEZ RODRIGUEZ</t>
+    <t>SEBASTIAN GUTIERREZ FIGUEROA</t>
+  </si>
+  <si>
+    <t>FOTO AVENTURAS</t>
+  </si>
+  <si>
+    <t>ALFONSO ARROYO TOSCANO</t>
+  </si>
+  <si>
+    <t>ESPIRITU SANTO</t>
   </si>
   <si>
     <t>MELISSA MARTINEZ HERNANDEZ</t>
   </si>
   <si>
-    <t>ERNESTO DE LEON MIRANDA</t>
+    <t>CARLOS MANUEL FLORES SANCHEZ</t>
+  </si>
+  <si>
+    <t>JORGE ENRIQUE SALCEDA GALVAN</t>
+  </si>
+  <si>
+    <t>RIGOBERTO ROMERO JORGE</t>
+  </si>
+  <si>
+    <t>LILIANA YUNUE MANRIQUEZ CASTRO</t>
   </si>
   <si>
     <t>ANDREA CORTES LOPEZ</t>
@@ -200,12 +302,12 @@
     <t>JUAN FERNANDO MACEDA GONZALEZ</t>
   </si>
   <si>
-    <t>MARIA ANGELICA MONGES AMADOR</t>
-  </si>
-  <si>
     <t>GLENDA YURIANA ARMENTA CORRAL</t>
   </si>
   <si>
+    <t>JONATHAN DE LA ROSA GONZALEZ</t>
+  </si>
+  <si>
     <t>ARTURO NAVA RODRIGUEZ</t>
   </si>
   <si>
@@ -221,58 +323,121 @@
     <t>MARCOS PORCHAS QUIJADA</t>
   </si>
   <si>
-    <t>WHALE SHARK</t>
-  </si>
-  <si>
     <t>ALFA PATRICIO GUEVARA</t>
   </si>
   <si>
     <t>LIMPIEZA</t>
   </si>
   <si>
-    <t xml:space="preserve">ELLIOT GEORGE MOSS BADRICK </t>
-  </si>
-  <si>
-    <t>DELFINES SJ</t>
+    <t>ERIK MIGUEL OLVERA GARCIA</t>
+  </si>
+  <si>
+    <t>EUNICE NORIEGA JIMENEZ</t>
+  </si>
+  <si>
+    <t>DAHIANA ALEJANDRA MARTINEZ ROMERO</t>
+  </si>
+  <si>
+    <t>NOEMI ORTIZ PINEDA</t>
   </si>
   <si>
     <t>JOSE CUAUHTEMOC VILLAVICENCIO PEREZ</t>
   </si>
   <si>
-    <t>ESPIRITU SANTO</t>
+    <t>VICTOR MANUEL COSIO POZO</t>
+  </si>
+  <si>
+    <t>CHECK IN SJ</t>
+  </si>
+  <si>
+    <t>ISELA GUADALUPE CORAZON ARRIAGA</t>
+  </si>
+  <si>
+    <t>RESERVACIONES</t>
   </si>
   <si>
     <t>PEDRO ANTONIO CASTILLO SANSORES</t>
   </si>
   <si>
+    <t>JAIME ALEJANDRO NORIEGA JIMENEZ</t>
+  </si>
+  <si>
     <t>MARIA LUISA HERNANDEZ GARCIA</t>
   </si>
   <si>
+    <t>JUAN PABLO RAMIREZ ALVAREZ</t>
+  </si>
+  <si>
+    <t>CHRISTIAN GIOVANNI NOVA JUAREZ</t>
+  </si>
+  <si>
+    <t>SNORKEL</t>
+  </si>
+  <si>
+    <t>ARANTZA DIAZ SANCHEZ</t>
+  </si>
+  <si>
+    <t>OSCAR MORALES MEJIA</t>
+  </si>
+  <si>
     <t>JAVIER ALVAREZ ROMAN</t>
   </si>
   <si>
+    <t>VICTOR MANUEL VILLEDA MUNOZ</t>
+  </si>
+  <si>
+    <t>LEONARDO MARTIN BENAVIDES GUTIERREZ</t>
+  </si>
+  <si>
     <t>FRANCISCO JAVIER RODRIGUEZ CONTRERAS</t>
   </si>
   <si>
     <t>JOSE DARIO COLLINS CASTILLO</t>
   </si>
   <si>
-    <t>FOTO Y VIDEO SJ</t>
-  </si>
-  <si>
     <t>AARON ANDRES DIAZ LEON</t>
   </si>
   <si>
     <t>PAUL CASTILLEJOS MACIEL</t>
   </si>
   <si>
+    <t>REY ARTURO PADILLA VARGAS</t>
+  </si>
+  <si>
+    <t>JUAN PABLO ANDRADE RAMOS</t>
+  </si>
+  <si>
     <t>RIGOBERTO BENITEZ SUSTERSIC</t>
   </si>
   <si>
+    <t>CESAR GABRIEL JIMENEZ NEVAREZ</t>
+  </si>
+  <si>
     <t>ELIZABETH MARIA SEYMOUR RAYGOZA</t>
   </si>
   <si>
-    <t xml:space="preserve">RACHEL DELL LACHINSKI </t>
+    <t>MONICA JHOVANA TORRES CELAYA</t>
+  </si>
+  <si>
+    <t>CHECK IN</t>
+  </si>
+  <si>
+    <t>JOSE CARLOS CORTES LOPEZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MANUELA DE DONA </t>
+  </si>
+  <si>
+    <t>MONTSERRAT CORONA FUENTES</t>
+  </si>
+  <si>
+    <t>HOSTESS SJ CAD</t>
+  </si>
+  <si>
+    <t>CHRISTIAN JUAN MOISES PAEZ VALENCIA</t>
+  </si>
+  <si>
+    <t>SERGIO TORRES LUJAN</t>
   </si>
   <si>
     <t>SILBIANO TAPIA NAVA</t>
@@ -281,6 +446,9 @@
     <t>VALERIA GALVEZ DE LA PENA</t>
   </si>
   <si>
+    <t>GABRIEL ZAZUETA MOULINIE</t>
+  </si>
+  <si>
     <t>JUAN CARLOS PINO PALACIO</t>
   </si>
   <si>
@@ -293,24 +461,48 @@
     <t>SIMON LOPEZ MONTOYA</t>
   </si>
   <si>
+    <t>LUIS ALBERTO CARRILLO GALLARDO</t>
+  </si>
+  <si>
     <t>JOSE LUIS CRUZ JIMENEZ</t>
   </si>
   <si>
     <t>EMMANUEL GONZALEZ MORA</t>
   </si>
   <si>
+    <t>JESUS ALBERTO ROMAN SORIA</t>
+  </si>
+  <si>
+    <t>ARTURO OSUNA LERMA</t>
+  </si>
+  <si>
+    <t>IATZIRY GABRIELA CORREA GOMEZ</t>
+  </si>
+  <si>
+    <t>TIENDA</t>
+  </si>
+  <si>
+    <t>ARANZA JAIMES MIRO</t>
+  </si>
+  <si>
     <t>SOFIA CAROLINA ARANA VALADEZ</t>
   </si>
   <si>
     <t>NICOLAS FRANCISCO RAMIREZ</t>
   </si>
   <si>
+    <t>VICENTE MANUEL TIJERINA IBARRA</t>
+  </si>
+  <si>
+    <t>JANETT ISELA HERNANDEZ ACEVEDO</t>
+  </si>
+  <si>
+    <t>ELIZABETH ONTIVEROS CAMACHO</t>
+  </si>
+  <si>
     <t>LEONARDO EMMANUEL CORTES ROMERO</t>
   </si>
   <si>
-    <t>LUIS FERNANDO PALOMERA DE LA BARRERA</t>
-  </si>
-  <si>
     <t>JORGE LUIS COLLINS ARAIZA</t>
   </si>
   <si>
@@ -320,61 +512,70 @@
     <t>MOUNTAIN BIKE</t>
   </si>
   <si>
+    <t>GLADYS MARIAH MONTEMAYOR PEREZ</t>
+  </si>
+  <si>
+    <t>ROLANDO JAVIER MONTEMAYOR PEREZ</t>
+  </si>
+  <si>
     <t>ALEJANDRA MUNOZ LEON</t>
   </si>
   <si>
     <t>COMEDOR SJ</t>
   </si>
   <si>
+    <t>JOSE MANUEL ARREDONDO LORENZO</t>
+  </si>
+  <si>
     <t>ALEJANDRO REYES SARABIA</t>
   </si>
   <si>
     <t>CHRISTIAN IVAN MONROY MORENO</t>
   </si>
   <si>
-    <t>OFF ROAD</t>
-  </si>
-  <si>
-    <t>JUAN ANTONIO OJEDA GARCIA</t>
+    <t>JORGE OMAR UNZON GERALDO</t>
+  </si>
+  <si>
+    <t>SILVIA RICHARDSON MEDINA</t>
+  </si>
+  <si>
+    <t>GABRIEL ALEJANDRO VELAZQUEZ VARGAS</t>
+  </si>
+  <si>
+    <t>ANA SOFIA ANGULO GARCIA</t>
+  </si>
+  <si>
+    <t>JOSE LUIS REYES RAMIREZ</t>
+  </si>
+  <si>
+    <t>ERIC POBLETE HERNANDEZ</t>
+  </si>
+  <si>
+    <t>FRANCISCO RAMON ARZATE KACHOK</t>
+  </si>
+  <si>
+    <t>AUGUSTO AGUIRRE MORALES</t>
+  </si>
+  <si>
+    <t>GONZALO CRUZ DIAZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUCERO ANGELICA DILLANES </t>
+  </si>
+  <si>
+    <t>LUIS MANUEL GONZALEZ RUIZ</t>
   </si>
   <si>
     <t>SEGURIDAD SJ</t>
   </si>
   <si>
-    <t>BRENDA NU¥O ROMERO</t>
-  </si>
-  <si>
-    <t>CHECK IN SJ</t>
-  </si>
-  <si>
-    <t>JORGE OMAR UNZON GERALDO</t>
-  </si>
-  <si>
-    <t>SILVIA RICHARDSON MEDINA</t>
-  </si>
-  <si>
-    <t>PEDRO GONZALEZ DE LA LUZ</t>
-  </si>
-  <si>
-    <t>HOSTESS SJ</t>
-  </si>
-  <si>
-    <t>MARCOS PALMA MU¥OZ</t>
-  </si>
-  <si>
-    <t>WHALE WATCHING TEMPORADA</t>
-  </si>
-  <si>
-    <t>AUGUSTO AGUIRRE MORALES</t>
-  </si>
-  <si>
-    <t>GONZALO CRUZ DIAZ</t>
-  </si>
-  <si>
-    <t>LUIS MANUEL GONZALEZ RUIZ</t>
-  </si>
-  <si>
     <t>ANGEL AMADOR CUEVAS</t>
+  </si>
+  <si>
+    <t>FLAVIO CESAR PEREZ GARCIA</t>
+  </si>
+  <si>
+    <t>FRANCISCO JAVIER DAVILA REZA</t>
   </si>
 </sst>
 </file>
@@ -728,7 +929,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="C19" sqref="C19"/>
@@ -766,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -775,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -784,7 +985,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -793,7 +994,7 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -802,16 +1003,16 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -820,16 +1021,16 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>251</v>
+        <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5">
         <v>6</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -838,16 +1039,16 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>365</v>
+        <v>208</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -856,16 +1057,16 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>389</v>
+        <v>251</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -874,16 +1075,16 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>485</v>
+        <v>329</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -892,16 +1093,16 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>502</v>
+        <v>333</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -910,16 +1111,16 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>561</v>
+        <v>365</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -928,16 +1129,16 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>630</v>
+        <v>366</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -946,16 +1147,16 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>659</v>
+        <v>389</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -964,16 +1165,16 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>670</v>
+        <v>448</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E13">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -982,16 +1183,16 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>696</v>
+        <v>458</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E14">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -1000,16 +1201,16 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>704</v>
+        <v>502</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E15">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -1018,16 +1219,16 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>709</v>
+        <v>519</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E16">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F16" s="2"/>
     </row>
@@ -1036,16 +1237,16 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>711</v>
+        <v>526</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E17">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F17" s="2"/>
     </row>
@@ -1054,16 +1255,16 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>714</v>
+        <v>549</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F18" s="2"/>
     </row>
@@ -1072,16 +1273,16 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <v>726</v>
+        <v>561</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F19" s="2"/>
     </row>
@@ -1090,16 +1291,16 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>751</v>
+        <v>582</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E20">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F20" s="2"/>
     </row>
@@ -1108,16 +1309,16 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>770</v>
+        <v>630</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E21">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -1126,16 +1327,16 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <v>785</v>
+        <v>634</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E22">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -1144,16 +1345,16 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>801</v>
+        <v>657</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F23" s="2"/>
     </row>
@@ -1162,16 +1363,16 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>853</v>
+        <v>659</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E24">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F24" s="2"/>
     </row>
@@ -1180,16 +1381,16 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>866</v>
+        <v>670</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F25" s="2"/>
     </row>
@@ -1198,16 +1399,16 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <v>905</v>
+        <v>675</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="E26">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -1216,16 +1417,16 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>916</v>
+        <v>694</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="E27">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F27" s="2"/>
     </row>
@@ -1234,16 +1435,16 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>922</v>
+        <v>696</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E28">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F28" s="2"/>
     </row>
@@ -1252,16 +1453,16 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <v>929</v>
+        <v>704</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E29">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F29" s="2"/>
     </row>
@@ -1270,16 +1471,16 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>938</v>
+        <v>709</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E30">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F30" s="2"/>
     </row>
@@ -1288,16 +1489,16 @@
         <v>1</v>
       </c>
       <c r="B31">
-        <v>953</v>
+        <v>711</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F31" s="2"/>
     </row>
@@ -1306,16 +1507,16 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>979</v>
+        <v>712</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="E32">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F32" s="2"/>
     </row>
@@ -1324,16 +1525,16 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>1000</v>
+        <v>713</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F33" s="2"/>
     </row>
@@ -1342,16 +1543,16 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>1004</v>
+        <v>714</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E34">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -1360,16 +1561,16 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>1008</v>
+        <v>726</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="E35">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F35" s="2"/>
     </row>
@@ -1378,16 +1579,16 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>1009</v>
+        <v>751</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F36" s="2"/>
     </row>
@@ -1396,16 +1597,16 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>1020</v>
+        <v>785</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E37">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F37" s="2"/>
     </row>
@@ -1414,16 +1615,16 @@
         <v>1</v>
       </c>
       <c r="B38">
-        <v>1026</v>
+        <v>801</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>55</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E38">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F38" s="2"/>
     </row>
@@ -1432,16 +1633,16 @@
         <v>1</v>
       </c>
       <c r="B39">
-        <v>1030</v>
+        <v>810</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F39" s="2"/>
     </row>
@@ -1450,16 +1651,16 @@
         <v>1</v>
       </c>
       <c r="B40">
-        <v>1052</v>
+        <v>833</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E40">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F40" s="2"/>
     </row>
@@ -1468,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>1083</v>
+        <v>836</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F41" s="2"/>
     </row>
@@ -1486,16 +1687,16 @@
         <v>1</v>
       </c>
       <c r="B42">
-        <v>1103</v>
+        <v>850</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E42">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F42" s="2"/>
     </row>
@@ -1504,16 +1705,16 @@
         <v>1</v>
       </c>
       <c r="B43">
-        <v>1114</v>
+        <v>853</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E43">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F43" s="2"/>
     </row>
@@ -1522,16 +1723,16 @@
         <v>1</v>
       </c>
       <c r="B44">
-        <v>1126</v>
+        <v>866</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="E44">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F44" s="2"/>
     </row>
@@ -1540,13 +1741,13 @@
         <v>1</v>
       </c>
       <c r="B45">
-        <v>1139</v>
+        <v>871</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -1558,16 +1759,16 @@
         <v>1</v>
       </c>
       <c r="B46">
-        <v>1147</v>
+        <v>905</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E46">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F46" s="2"/>
     </row>
@@ -1576,16 +1777,16 @@
         <v>1</v>
       </c>
       <c r="B47">
-        <v>1152</v>
+        <v>916</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E47">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F47" s="2"/>
     </row>
@@ -1594,16 +1795,16 @@
         <v>1</v>
       </c>
       <c r="B48">
-        <v>1153</v>
+        <v>922</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E48">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F48" s="2"/>
     </row>
@@ -1612,16 +1813,16 @@
         <v>1</v>
       </c>
       <c r="B49">
-        <v>1158</v>
+        <v>923</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E49">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F49" s="2"/>
     </row>
@@ -1630,16 +1831,16 @@
         <v>1</v>
       </c>
       <c r="B50">
-        <v>1171</v>
+        <v>929</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E50">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F50" s="2"/>
     </row>
@@ -1648,16 +1849,16 @@
         <v>1</v>
       </c>
       <c r="B51">
-        <v>1180</v>
+        <v>938</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="E51">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F51" s="2"/>
     </row>
@@ -1666,16 +1867,16 @@
         <v>1</v>
       </c>
       <c r="B52">
-        <v>1199</v>
+        <v>953</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F52" s="2"/>
     </row>
@@ -1684,16 +1885,16 @@
         <v>1</v>
       </c>
       <c r="B53">
-        <v>1204</v>
+        <v>962</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E53">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F53" s="2"/>
     </row>
@@ -1702,16 +1903,16 @@
         <v>1</v>
       </c>
       <c r="B54">
-        <v>1216</v>
+        <v>979</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E54">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F54" s="2"/>
     </row>
@@ -1720,16 +1921,16 @@
         <v>1</v>
       </c>
       <c r="B55">
-        <v>1223</v>
+        <v>1000</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2"/>
     </row>
@@ -1738,16 +1939,16 @@
         <v>1</v>
       </c>
       <c r="B56">
-        <v>1235</v>
+        <v>1004</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="E56">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F56" s="2"/>
     </row>
@@ -1756,16 +1957,16 @@
         <v>1</v>
       </c>
       <c r="B57">
-        <v>1244</v>
+        <v>1008</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F57" s="2"/>
     </row>
@@ -1774,16 +1975,16 @@
         <v>1</v>
       </c>
       <c r="B58">
-        <v>1245</v>
+        <v>1009</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="E58">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F58" s="2"/>
     </row>
@@ -1792,16 +1993,16 @@
         <v>1</v>
       </c>
       <c r="B59">
-        <v>1249</v>
+        <v>1010</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>68</v>
+        <v>27</v>
       </c>
       <c r="E59">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F59" s="2"/>
     </row>
@@ -1810,16 +2011,16 @@
         <v>1</v>
       </c>
       <c r="B60">
-        <v>1250</v>
+        <v>1025</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="E60">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F60" s="2"/>
     </row>
@@ -1828,16 +2029,16 @@
         <v>1</v>
       </c>
       <c r="B61">
-        <v>1272</v>
+        <v>1026</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>83</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="E61">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F61" s="2"/>
     </row>
@@ -1846,16 +2047,16 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>1293</v>
+        <v>1038</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E62">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F62" s="2"/>
     </row>
@@ -1864,13 +2065,13 @@
         <v>1</v>
       </c>
       <c r="B63">
-        <v>1337</v>
+        <v>1045</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="E63">
         <v>4</v>
@@ -1882,16 +2083,16 @@
         <v>1</v>
       </c>
       <c r="B64">
-        <v>1345</v>
+        <v>1052</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="E64">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1899,16 +2100,16 @@
         <v>1</v>
       </c>
       <c r="B65">
-        <v>1363</v>
+        <v>1058</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E65">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1916,16 +2117,16 @@
         <v>1</v>
       </c>
       <c r="B66">
-        <v>1374</v>
+        <v>1066</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="E66">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1933,16 +2134,16 @@
         <v>1</v>
       </c>
       <c r="B67">
-        <v>1379</v>
+        <v>1079</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E67">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1950,16 +2151,16 @@
         <v>1</v>
       </c>
       <c r="B68">
-        <v>1380</v>
+        <v>1101</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E68">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1967,16 +2168,16 @@
         <v>1</v>
       </c>
       <c r="B69">
-        <v>1381</v>
+        <v>1103</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E69">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1984,16 +2185,16 @@
         <v>1</v>
       </c>
       <c r="B70">
-        <v>1386</v>
+        <v>1114</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E70">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -2001,16 +2202,16 @@
         <v>1</v>
       </c>
       <c r="B71">
-        <v>1387</v>
+        <v>1139</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="E71">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2018,16 +2219,16 @@
         <v>1</v>
       </c>
       <c r="B72">
-        <v>1411</v>
+        <v>1146</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72">
         <v>6</v>
-      </c>
-      <c r="E72">
-        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2035,16 +2236,16 @@
         <v>1</v>
       </c>
       <c r="B73">
-        <v>1419</v>
+        <v>1147</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E73">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2052,16 +2253,16 @@
         <v>1</v>
       </c>
       <c r="B74">
-        <v>1433</v>
+        <v>1152</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E74">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2069,16 +2270,16 @@
         <v>1</v>
       </c>
       <c r="B75">
-        <v>1434</v>
+        <v>1153</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E75">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -2086,16 +2287,16 @@
         <v>1</v>
       </c>
       <c r="B76">
-        <v>1441</v>
+        <v>1158</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E76">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2103,16 +2304,16 @@
         <v>1</v>
       </c>
       <c r="B77">
-        <v>1444</v>
+        <v>1171</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="E77">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2120,16 +2321,16 @@
         <v>1</v>
       </c>
       <c r="B78">
-        <v>1469</v>
+        <v>1180</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E78">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -2137,16 +2338,16 @@
         <v>1</v>
       </c>
       <c r="B79">
-        <v>1471</v>
+        <v>1182</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="E79">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2154,13 +2355,13 @@
         <v>1</v>
       </c>
       <c r="B80">
-        <v>1473</v>
+        <v>1184</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -2171,16 +2372,16 @@
         <v>1</v>
       </c>
       <c r="B81">
-        <v>1475</v>
+        <v>1195</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="E81">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2188,16 +2389,16 @@
         <v>1</v>
       </c>
       <c r="B82">
-        <v>1477</v>
+        <v>1202</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="E82">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2205,16 +2406,16 @@
         <v>1</v>
       </c>
       <c r="B83">
-        <v>1478</v>
+        <v>1204</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="E83">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2222,16 +2423,16 @@
         <v>1</v>
       </c>
       <c r="B84">
-        <v>1488</v>
+        <v>1213</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>18</v>
+        <v>110</v>
       </c>
       <c r="E84">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2239,16 +2440,16 @@
         <v>1</v>
       </c>
       <c r="B85">
-        <v>1499</v>
+        <v>1214</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D85" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="E85">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2256,16 +2457,16 @@
         <v>1</v>
       </c>
       <c r="B86">
-        <v>1503</v>
+        <v>1216</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>115</v>
+        <v>12</v>
       </c>
       <c r="E86">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2273,16 +2474,16 @@
         <v>1</v>
       </c>
       <c r="B87">
-        <v>1506</v>
+        <v>1217</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="E87">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2290,16 +2491,16 @@
         <v>1</v>
       </c>
       <c r="B88">
-        <v>1507</v>
+        <v>1223</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>105</v>
+        <v>12</v>
       </c>
       <c r="E88">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2307,16 +2508,16 @@
         <v>1</v>
       </c>
       <c r="B89">
-        <v>1519</v>
+        <v>1228</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>107</v>
+        <v>27</v>
       </c>
       <c r="E89">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2324,16 +2525,1070 @@
         <v>1</v>
       </c>
       <c r="B90">
+        <v>1230</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="B91">
+        <v>1231</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>1232</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>1235</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E93">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>1240</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95">
+        <v>1</v>
+      </c>
+      <c r="B95">
+        <v>1243</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>1244</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>1245</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E97">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98">
+        <v>1249</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E98">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99">
+        <v>1</v>
+      </c>
+      <c r="B99">
+        <v>1250</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100">
+        <v>1</v>
+      </c>
+      <c r="B100">
+        <v>1258</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101">
+        <v>1</v>
+      </c>
+      <c r="B101">
+        <v>1259</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102">
+        <v>1</v>
+      </c>
+      <c r="B102">
+        <v>1272</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E102">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103">
+        <v>1</v>
+      </c>
+      <c r="B103">
+        <v>1274</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104">
+        <v>1</v>
+      </c>
+      <c r="B104">
+        <v>1293</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105">
+        <v>1</v>
+      </c>
+      <c r="B105">
+        <v>1296</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E105">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106">
+        <v>1</v>
+      </c>
+      <c r="B106">
+        <v>1306</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107">
+        <v>1</v>
+      </c>
+      <c r="B107">
+        <v>1321</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108">
+        <v>1</v>
+      </c>
+      <c r="B108">
+        <v>1325</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E108">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109">
+        <v>1</v>
+      </c>
+      <c r="B109">
+        <v>1335</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110">
+        <v>1</v>
+      </c>
+      <c r="B110">
+        <v>1341</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111">
+        <v>1</v>
+      </c>
+      <c r="B111">
+        <v>1345</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112">
+        <v>1</v>
+      </c>
+      <c r="B112">
+        <v>1363</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E112">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="B113">
+        <v>1366</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E113">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114">
+        <v>1</v>
+      </c>
+      <c r="B114">
+        <v>1374</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E114">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115">
+        <v>1</v>
+      </c>
+      <c r="B115">
+        <v>1379</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116">
+        <v>1</v>
+      </c>
+      <c r="B116">
+        <v>1380</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E116">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117">
+        <v>1</v>
+      </c>
+      <c r="B117">
+        <v>1381</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E117">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="B118">
+        <v>1385</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E118">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119">
+        <v>1</v>
+      </c>
+      <c r="B119">
+        <v>1386</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E119">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120">
+        <v>1</v>
+      </c>
+      <c r="B120">
+        <v>1387</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E120">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121">
+        <v>1</v>
+      </c>
+      <c r="B121">
+        <v>1390</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122">
+        <v>1</v>
+      </c>
+      <c r="B122">
+        <v>1398</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E122">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123">
+        <v>1</v>
+      </c>
+      <c r="B123">
+        <v>1400</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124">
+        <v>1</v>
+      </c>
+      <c r="B124">
+        <v>1409</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125">
+        <v>1</v>
+      </c>
+      <c r="B125">
+        <v>1411</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126">
+        <v>1419</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E126">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127">
+        <v>1</v>
+      </c>
+      <c r="B127">
+        <v>1420</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E127">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128">
+        <v>1</v>
+      </c>
+      <c r="B128">
+        <v>1424</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E128">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129">
+        <v>1</v>
+      </c>
+      <c r="B129">
+        <v>1432</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130">
+        <v>1</v>
+      </c>
+      <c r="B130">
+        <v>1433</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131">
+        <v>1</v>
+      </c>
+      <c r="B131">
+        <v>1441</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132">
+        <v>1</v>
+      </c>
+      <c r="B132">
+        <v>1444</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E132">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133">
+        <v>1</v>
+      </c>
+      <c r="B133">
+        <v>1450</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E133">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134">
+        <v>1</v>
+      </c>
+      <c r="B134">
+        <v>1468</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135">
+        <v>1469</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E135">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136">
+        <v>1</v>
+      </c>
+      <c r="B136">
+        <v>1470</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E136">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137">
+        <v>1</v>
+      </c>
+      <c r="B137">
+        <v>1471</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E137">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138">
+        <v>1</v>
+      </c>
+      <c r="B138">
+        <v>1473</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E138">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139">
+        <v>1</v>
+      </c>
+      <c r="B139">
+        <v>1478</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E139">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140">
+        <v>1</v>
+      </c>
+      <c r="B140">
+        <v>1488</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E140">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141">
+        <v>1</v>
+      </c>
+      <c r="B141">
+        <v>1490</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>1494</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>1495</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>1496</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E144">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>1505</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>1506</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E146">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>1507</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>1512</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E148">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>1519</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E149">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
         <v>1526</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E90">
-        <v>8</v>
+      <c r="C150" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E150">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>1528</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E151">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>1532</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E152">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>